<commit_message>
minor updates to calibrator spreadsheet utilities for conductivity & turbidity
</commit_message>
<xml_diff>
--- a/utilities/CalibrationProtocolSpreadsheet/Y511-Turbidity-Calibrator.xlsx
+++ b/utilities/CalibrationProtocolSpreadsheet/Y511-Turbidity-Calibrator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaufdenkampe/Documents/Arduino/YosemitechModbus/utilities/CalibrationProtocolSpreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99C9775-F79B-7E41-A34A-F0102125FC75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C546F8B-7F64-CD4C-88FA-A7CFACC86CC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="-21140" windowWidth="33260" windowHeight="20340" xr2:uid="{A01D2E8A-3A02-234A-9567-63BD2965B45A}"/>
+    <workbookView xWindow="1000" yWindow="1280" windowWidth="33260" windowHeight="20340" xr2:uid="{A01D2E8A-3A02-234A-9567-63BD2965B45A}"/>
   </bookViews>
   <sheets>
     <sheet name="YL09-blank" sheetId="8" r:id="rId1"/>
@@ -20,15 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
-  <si>
-    <t>mS/cm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Average</t>
   </si>
@@ -123,9 +129,6 @@
     <t>Standard practice is for calibration curves to have the known reference values on the X-axis, because they are the "independent" variable.</t>
   </si>
   <si>
-    <t>YosemiTech puts the measured values on the X-axis, despite it being the "independent variable". Many other well-known sensor companies also follow this practice, even though it does not technically follow statistical best practice.</t>
-  </si>
-  <si>
     <t>predicted Y</t>
   </si>
   <si>
@@ -141,9 +144,6 @@
     <t>3. Fill in reference standard known values.</t>
   </si>
   <si>
-    <t>4."GET Cond" &amp; paste measured values for each standard.</t>
-  </si>
-  <si>
     <t>6. Re-SET "User Coefficients" to new calibration values.</t>
   </si>
   <si>
@@ -153,9 +153,6 @@
     <t xml:space="preserve"> Delete green values in pale yellow cells D25:E28</t>
   </si>
   <si>
-    <t>intercept in mS/cm</t>
-  </si>
-  <si>
     <t>Paste these blue values into Modbus Runner and hit "SET".</t>
   </si>
   <si>
@@ -178,6 +175,21 @@
   </si>
   <si>
     <t>NTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YosemiTech puts the measured values on the X-axis, despite it being the "independent variable". </t>
+  </si>
+  <si>
+    <t>Many other well-known sensor companies also follow this practice, even though it does not technically follow statistical best practice.</t>
+  </si>
+  <si>
+    <t>intercept in NTU or FTU</t>
+  </si>
+  <si>
+    <t>NTU or FTU</t>
+  </si>
+  <si>
+    <t>4."GET Turb" &amp; paste measured values for each standard.</t>
   </si>
 </sst>
 </file>
@@ -1533,7 +1545,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1554,15 +1566,15 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
@@ -1577,43 +1589,43 @@
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="7"/>
       <c r="I3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="7"/>
       <c r="L3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="7"/>
       <c r="O3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
@@ -1628,47 +1640,47 @@
     </row>
     <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="E5" s="3" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="23"/>
-      <c r="K5" s="23" t="s">
-        <v>0</v>
+      <c r="K5" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M5" s="23"/>
-      <c r="N5" s="23" t="s">
-        <v>0</v>
+      <c r="N5" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P5" s="23"/>
-      <c r="Q5" s="23" t="s">
-        <v>0</v>
+      <c r="Q5" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="13"/>
       <c r="E6" s="7"/>
@@ -1696,7 +1708,7 @@
     </row>
     <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1711,7 +1723,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="7"/>
       <c r="E9" s="7"/>
@@ -1727,7 +1739,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="7"/>
       <c r="E10" s="7"/>
@@ -1743,10 +1755,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1761,11 +1773,11 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -1780,11 +1792,11 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -1811,7 +1823,7 @@
     </row>
     <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -1826,7 +1838,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="15">
         <v>1</v>
@@ -1836,14 +1848,14 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="9" t="e">
         <f>AVERAGE(E6:E15)</f>
@@ -1889,7 +1901,7 @@
     <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="C18" s="12"/>
       <c r="D18" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="9" t="e">
         <f>STDEV(E6:E15)</f>
@@ -1934,11 +1946,11 @@
     </row>
     <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="11" t="e">
         <f>E18/E17</f>
@@ -1983,7 +1995,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1995,10 +2007,10 @@
     </row>
     <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
@@ -2007,45 +2019,45 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="23" t="s">
-        <v>15</v>
-      </c>
       <c r="T23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="U23" s="23" t="s">
         <v>14</v>
-      </c>
-      <c r="U23" s="23" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="T24" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U24" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.15">
@@ -2066,7 +2078,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="K25" s="8" t="e">
-        <f>(E25+$F$32) * $F$31</f>
+        <f>$F$31 * E25 + $F$32</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T25" s="8" t="e">
@@ -2080,7 +2092,7 @@
     </row>
     <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E26" s="24" t="e">
         <f t="shared" si="0"/>
@@ -2099,7 +2111,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="K26" s="8" t="e">
-        <f t="shared" ref="K26:K28" si="2">(E26+$F$32) * $F$31</f>
+        <f t="shared" ref="K26:K28" si="2">$F$31 * E26 + $F$32</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T26" s="8" t="e">
@@ -2113,7 +2125,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E27" s="24" t="e">
         <f t="shared" si="0"/>
@@ -2176,96 +2188,91 @@
     </row>
     <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="26" t="e">
         <f>F31</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" s="9" t="e">
         <f>SLOPE($F$25:$F$28,$E$25:$E$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="26" t="e">
-        <f>F34</f>
+        <f>F32</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="9" t="e">
         <f>INTERCEPT($F$25:$F$28,$E$25:$E$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="F33" s="25"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="T33" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34" s="18"/>
-      <c r="E34" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="9" t="e">
-        <f>F32/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="E34" s="12"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="E37" s="12"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="E38" s="12"/>
     </row>
   </sheetData>

</xml_diff>